<commit_message>
feat: now can crawl XHR & static page envenforcement file items
</commit_message>
<xml_diff>
--- a/entryUrls_minimal2.xlsx
+++ b/entryUrls_minimal2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/k/Repos/envEnforcementData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61BBD538-CFC8-4447-AB9F-F50615B8DF55}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52CE88F8-7061-8546-93B3-469A80B32EF4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="14140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -139,14 +139,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -189,18 +182,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -214,44 +201,38 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -535,39 +516,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="4" width="9" style="7"/>
-    <col min="5" max="5" width="60.1640625" style="7" customWidth="1"/>
-    <col min="6" max="6" width="127" style="7" customWidth="1"/>
-    <col min="7" max="10" width="9" style="7"/>
-    <col min="11" max="11" width="9" style="7" customWidth="1"/>
-    <col min="12" max="16384" width="9" style="7"/>
+    <col min="1" max="3" width="9" style="6"/>
+    <col min="4" max="4" width="45" style="6" customWidth="1"/>
+    <col min="5" max="5" width="60.1640625" style="6" customWidth="1"/>
+    <col min="6" max="6" width="127" style="6" customWidth="1"/>
+    <col min="7" max="10" width="9" style="6"/>
+    <col min="11" max="11" width="9" style="6" customWidth="1"/>
+    <col min="12" max="16384" width="9" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>25</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -587,31 +569,31 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="H2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="I2" s="9" t="s">
         <v>14</v>
       </c>
       <c r="J2" s="2" t="s">
@@ -620,22 +602,22 @@
       <c r="K2" s="2"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="9" t="s">
         <v>19</v>
       </c>
       <c r="G3" s="2"/>
@@ -645,153 +627,53 @@
       <c r="K3" s="2"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="3" t="s">
         <v>23</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="H4" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="I4" s="10" t="s">
+      <c r="I4" s="9" t="s">
         <v>14</v>
       </c>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="6"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" s="6"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="6"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" s="6"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" s="6"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-    </row>
+    <row r="5" spans="1:11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="1:11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="7" spans="1:11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="9" spans="1:11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="17" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="19" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="20" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="21" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>

</xml_diff>